<commit_message>
Add changes suggested by ELAVI team
</commit_message>
<xml_diff>
--- a/params/deshmuk_calculations.xlsx
+++ b/params/deshmuk_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\david\anus\params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801402ED-7BC6-45AA-875F-757DEBF27368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970B377D-8B5C-4B9F-9E49-543497AEB005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45105E01-CB45-454B-A410-687B1C9BDE7E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{45105E01-CB45-454B-A410-687B1C9BDE7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>CD4 distribution</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>HGAIN to anal cancer (calibrated)</t>
+  </si>
+  <si>
+    <t>Source: ELAVI</t>
+  </si>
+  <si>
+    <t>Utilities</t>
   </si>
 </sst>
 </file>
@@ -105,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +121,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,9 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7785D7C-A208-42DB-AC98-6E17F53E3E7A}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,6 +489,9 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
@@ -486,11 +509,14 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>0.11650000000000001</v>
       </c>
       <c r="C2">
         <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.94</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -509,11 +535,14 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.29730000000000001</v>
       </c>
       <c r="C3">
         <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.87</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -532,11 +561,14 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.58620000000000005</v>
       </c>
       <c r="C4">
         <v>0.13800000000000001</v>
+      </c>
+      <c r="D4">
+        <v>0.8</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -570,6 +602,10 @@
         <f>B2*C2+B3*C3+B4*C4</f>
         <v>0.10282700000000002</v>
       </c>
+      <c r="D6" s="1">
+        <f>B2*D2+B3*D3+B4*D4</f>
+        <v>0.837121</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F7" t="s">
@@ -579,9 +615,82 @@
         <v>0.23499999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.83898305084745761</v>
+      </c>
+      <c r="C13">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.14689265536723164</v>
+      </c>
+      <c r="C14">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D14">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.4124293785310734E-2</v>
+      </c>
+      <c r="C15">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <f>B13*C13+B14*C14+B15*C15</f>
+        <v>5.4200564971751408E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <f>B13*D13+B14*D14+B15*D15</f>
+        <v>0.92774011299435022</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>